<commit_message>
add more spike sorting and channel data
</commit_message>
<xml_diff>
--- a/spike sorting notes.xlsx
+++ b/spike sorting notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\MATLAB\gratings-task-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A0B0E6-486B-4B68-AEA1-5B9B74D3F798}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DE30BC-63F3-415C-8060-3FF1F7B4B9E5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{F5215BA6-879C-42E2-A238-7256D4555DD7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{F5215BA6-879C-42E2-A238-7256D4555DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Unit Info" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2318" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2366" uniqueCount="278">
   <si>
     <t>Session</t>
   </si>
@@ -846,6 +846,21 @@
   <si>
     <t>M20170529</t>
   </si>
+  <si>
+    <t>Broad triphasic waveform, middle third only</t>
+  </si>
+  <si>
+    <t>Broad triphasic waveform</t>
+  </si>
+  <si>
+    <t>No clear unit, but clear ISI pattern</t>
+  </si>
+  <si>
+    <t>Negative only waveform</t>
+  </si>
+  <si>
+    <t>Separated only for first quarter</t>
+  </si>
 </sst>
 </file>
 
@@ -1209,10 +1224,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{991F1F63-41CC-4425-B140-2A823B1406A8}">
-  <dimension ref="A1:F1760"/>
+  <dimension ref="A1:F1792"/>
   <sheetViews>
-    <sheetView topLeftCell="A1625" workbookViewId="0">
-      <selection activeCell="A1649" sqref="A1649"/>
+    <sheetView tabSelected="1" topLeftCell="A1621" workbookViewId="0">
+      <selection activeCell="A1642" sqref="A1642:A1673"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30605,7 +30620,7 @@
         <v>272</v>
       </c>
       <c r="B1642">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C1642">
         <v>0</v>
@@ -30622,7 +30637,7 @@
         <v>272</v>
       </c>
       <c r="B1643">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C1643">
         <v>1</v>
@@ -30631,7 +30646,10 @@
         <v>1</v>
       </c>
       <c r="E1643">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F1643" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="1644" spans="1:6" x14ac:dyDescent="0.25">
@@ -30639,7 +30657,7 @@
         <v>272</v>
       </c>
       <c r="B1644">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C1644">
         <v>2</v>
@@ -30648,7 +30666,10 @@
         <v>1</v>
       </c>
       <c r="E1644">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F1644" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="1645" spans="1:6" x14ac:dyDescent="0.25">
@@ -30656,7 +30677,7 @@
         <v>272</v>
       </c>
       <c r="B1645">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C1645">
         <v>0</v>
@@ -30666,6 +30687,9 @@
       </c>
       <c r="E1645">
         <v>0</v>
+      </c>
+      <c r="F1645" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="1646" spans="1:6" x14ac:dyDescent="0.25">
@@ -30673,16 +30697,16 @@
         <v>272</v>
       </c>
       <c r="B1646">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C1646">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1646">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1646">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1647" spans="1:6" x14ac:dyDescent="0.25">
@@ -30690,16 +30714,19 @@
         <v>272</v>
       </c>
       <c r="B1647">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C1647">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1647">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1647">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="F1647" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="1648" spans="1:6" x14ac:dyDescent="0.25">
@@ -30707,10 +30734,10 @@
         <v>272</v>
       </c>
       <c r="B1648">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C1648">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1648">
         <v>0</v>
@@ -30719,7 +30746,7 @@
         <v>3</v>
       </c>
       <c r="F1648" t="s">
-        <v>263</v>
+        <v>276</v>
       </c>
     </row>
     <row r="1649" spans="1:6" x14ac:dyDescent="0.25">
@@ -30727,19 +30754,19 @@
         <v>272</v>
       </c>
       <c r="B1649">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C1649">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D1649">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1649">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F1649" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1650" spans="1:6" x14ac:dyDescent="0.25">
@@ -30747,7 +30774,7 @@
         <v>272</v>
       </c>
       <c r="B1650">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C1650">
         <v>0</v>
@@ -30767,7 +30794,7 @@
         <v>272</v>
       </c>
       <c r="B1651">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C1651">
         <v>0</v>
@@ -30777,6 +30804,9 @@
       </c>
       <c r="E1651">
         <v>0</v>
+      </c>
+      <c r="F1651" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="1652" spans="1:6" x14ac:dyDescent="0.25">
@@ -30784,16 +30814,19 @@
         <v>272</v>
       </c>
       <c r="B1652">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C1652">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1652">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1652">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="F1652" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="1653" spans="1:6" x14ac:dyDescent="0.25">
@@ -30801,7 +30834,7 @@
         <v>272</v>
       </c>
       <c r="B1653">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C1653">
         <v>0</v>
@@ -30811,6 +30844,9 @@
       </c>
       <c r="E1653">
         <v>0</v>
+      </c>
+      <c r="F1653" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="1654" spans="1:6" x14ac:dyDescent="0.25">
@@ -30818,16 +30854,19 @@
         <v>272</v>
       </c>
       <c r="B1654">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C1654">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1654">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1654">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="F1654" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="1655" spans="1:6" x14ac:dyDescent="0.25">
@@ -30835,16 +30874,16 @@
         <v>272</v>
       </c>
       <c r="B1655">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C1655">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1655">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1655">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1656" spans="1:6" x14ac:dyDescent="0.25">
@@ -30852,19 +30891,16 @@
         <v>272</v>
       </c>
       <c r="B1656">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C1656">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D1656">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1656">
         <v>2</v>
-      </c>
-      <c r="F1656" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="1657" spans="1:6" x14ac:dyDescent="0.25">
@@ -30872,16 +30908,16 @@
         <v>272</v>
       </c>
       <c r="B1657">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C1657">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1657">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1657">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1658" spans="1:6" x14ac:dyDescent="0.25">
@@ -30889,16 +30925,19 @@
         <v>272</v>
       </c>
       <c r="B1658">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C1658">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1658">
         <v>1</v>
       </c>
       <c r="E1658">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="F1658" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="1659" spans="1:6" x14ac:dyDescent="0.25">
@@ -30906,16 +30945,16 @@
         <v>272</v>
       </c>
       <c r="B1659">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C1659">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1659">
         <v>1</v>
       </c>
       <c r="E1659">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1660" spans="1:6" x14ac:dyDescent="0.25">
@@ -30923,16 +30962,16 @@
         <v>272</v>
       </c>
       <c r="B1660">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C1660">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D1660">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1660">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1661" spans="1:6" x14ac:dyDescent="0.25">
@@ -30940,19 +30979,19 @@
         <v>272</v>
       </c>
       <c r="B1661">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C1661">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1661">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1661">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F1661" t="s">
-        <v>271</v>
+        <v>12</v>
       </c>
     </row>
     <row r="1662" spans="1:6" x14ac:dyDescent="0.25">
@@ -30960,16 +30999,19 @@
         <v>272</v>
       </c>
       <c r="B1662">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C1662">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1662">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1662">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="F1662" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="1663" spans="1:6" x14ac:dyDescent="0.25">
@@ -30977,16 +31019,16 @@
         <v>272</v>
       </c>
       <c r="B1663">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C1663">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D1663">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1663">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1664" spans="1:6" x14ac:dyDescent="0.25">
@@ -30994,19 +31036,16 @@
         <v>272</v>
       </c>
       <c r="B1664">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C1664">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D1664">
         <v>1</v>
       </c>
       <c r="E1664">
-        <v>2</v>
-      </c>
-      <c r="F1664" t="s">
-        <v>202</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1665" spans="1:6" x14ac:dyDescent="0.25">
@@ -31014,16 +31053,19 @@
         <v>272</v>
       </c>
       <c r="B1665">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C1665">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1665">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1665">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="F1665" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="1666" spans="1:6" x14ac:dyDescent="0.25">
@@ -31031,19 +31073,16 @@
         <v>272</v>
       </c>
       <c r="B1666">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C1666">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1666">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1666">
-        <v>5</v>
-      </c>
-      <c r="F1666" t="s">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1667" spans="1:6" x14ac:dyDescent="0.25">
@@ -31051,19 +31090,16 @@
         <v>272</v>
       </c>
       <c r="B1667">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C1667">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1667">
         <v>1</v>
       </c>
       <c r="E1667">
-        <v>3</v>
-      </c>
-      <c r="F1667" t="s">
-        <v>269</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1668" spans="1:6" x14ac:dyDescent="0.25">
@@ -31071,7 +31107,7 @@
         <v>272</v>
       </c>
       <c r="B1668">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C1668">
         <v>0</v>
@@ -31088,7 +31124,7 @@
         <v>272</v>
       </c>
       <c r="B1669">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C1669">
         <v>1</v>
@@ -31097,7 +31133,7 @@
         <v>1</v>
       </c>
       <c r="E1669">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1670" spans="1:6" x14ac:dyDescent="0.25">
@@ -31105,16 +31141,16 @@
         <v>272</v>
       </c>
       <c r="B1670">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C1670">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1670">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1670">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1671" spans="1:6" x14ac:dyDescent="0.25">
@@ -31122,16 +31158,16 @@
         <v>272</v>
       </c>
       <c r="B1671">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C1671">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1671">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1671">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1672" spans="1:6" x14ac:dyDescent="0.25">
@@ -31139,16 +31175,19 @@
         <v>272</v>
       </c>
       <c r="B1672">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C1672">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1672">
         <v>1</v>
       </c>
       <c r="E1672">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="F1672" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="1673" spans="1:6" x14ac:dyDescent="0.25">
@@ -31156,16 +31195,16 @@
         <v>272</v>
       </c>
       <c r="B1673">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C1673">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1673">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1673">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1674" spans="1:6" x14ac:dyDescent="0.25">
@@ -31173,16 +31212,16 @@
         <v>272</v>
       </c>
       <c r="B1674">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C1674">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1674">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1674">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1675" spans="1:6" x14ac:dyDescent="0.25">
@@ -31190,16 +31229,16 @@
         <v>272</v>
       </c>
       <c r="B1675">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C1675">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1675">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1675">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1676" spans="1:6" x14ac:dyDescent="0.25">
@@ -31207,16 +31246,16 @@
         <v>272</v>
       </c>
       <c r="B1676">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C1676">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1676">
         <v>1</v>
       </c>
       <c r="E1676">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1677" spans="1:6" x14ac:dyDescent="0.25">
@@ -31224,7 +31263,7 @@
         <v>272</v>
       </c>
       <c r="B1677">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C1677">
         <v>0</v>
@@ -31234,9 +31273,6 @@
       </c>
       <c r="E1677">
         <v>0</v>
-      </c>
-      <c r="F1677" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="1678" spans="1:6" x14ac:dyDescent="0.25">
@@ -31244,16 +31280,16 @@
         <v>272</v>
       </c>
       <c r="B1678">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C1678">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1678">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1678">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1679" spans="1:6" x14ac:dyDescent="0.25">
@@ -31261,16 +31297,16 @@
         <v>272</v>
       </c>
       <c r="B1679">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C1679">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1679">
         <v>1</v>
       </c>
       <c r="E1679">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1680" spans="1:6" x14ac:dyDescent="0.25">
@@ -31278,16 +31314,19 @@
         <v>272</v>
       </c>
       <c r="B1680">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C1680">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D1680">
         <v>0</v>
       </c>
       <c r="E1680">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="F1680" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="1681" spans="1:6" x14ac:dyDescent="0.25">
@@ -31295,16 +31334,19 @@
         <v>272</v>
       </c>
       <c r="B1681">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C1681">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D1681">
         <v>1</v>
       </c>
       <c r="E1681">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F1681" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="1682" spans="1:6" x14ac:dyDescent="0.25">
@@ -31312,7 +31354,7 @@
         <v>272</v>
       </c>
       <c r="B1682">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C1682">
         <v>0</v>
@@ -31322,6 +31364,9 @@
       </c>
       <c r="E1682">
         <v>0</v>
+      </c>
+      <c r="F1682" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="1683" spans="1:6" x14ac:dyDescent="0.25">
@@ -31329,16 +31374,16 @@
         <v>272</v>
       </c>
       <c r="B1683">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C1683">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1683">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1683">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1684" spans="1:6" x14ac:dyDescent="0.25">
@@ -31346,16 +31391,16 @@
         <v>272</v>
       </c>
       <c r="B1684">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C1684">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1684">
         <v>1</v>
       </c>
       <c r="E1684">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1685" spans="1:6" x14ac:dyDescent="0.25">
@@ -31363,19 +31408,16 @@
         <v>272</v>
       </c>
       <c r="B1685">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C1685">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D1685">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1685">
-        <v>3</v>
-      </c>
-      <c r="F1685" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1686" spans="1:6" x14ac:dyDescent="0.25">
@@ -31383,10 +31425,10 @@
         <v>272</v>
       </c>
       <c r="B1686">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C1686">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D1686">
         <v>1</v>
@@ -31400,19 +31442,16 @@
         <v>272</v>
       </c>
       <c r="B1687">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C1687">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D1687">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1687">
         <v>3</v>
-      </c>
-      <c r="F1687" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="1688" spans="1:6" x14ac:dyDescent="0.25">
@@ -31420,16 +31459,19 @@
         <v>272</v>
       </c>
       <c r="B1688">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C1688">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D1688">
         <v>0</v>
       </c>
       <c r="E1688">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="F1688" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="1689" spans="1:6" x14ac:dyDescent="0.25">
@@ -31437,19 +31479,16 @@
         <v>272</v>
       </c>
       <c r="B1689">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C1689">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1689">
         <v>0</v>
       </c>
       <c r="E1689">
-        <v>5</v>
-      </c>
-      <c r="F1689" t="s">
-        <v>263</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1690" spans="1:6" x14ac:dyDescent="0.25">
@@ -31457,19 +31496,16 @@
         <v>272</v>
       </c>
       <c r="B1690">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C1690">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1690">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1690">
-        <v>5</v>
-      </c>
-      <c r="F1690" t="s">
-        <v>264</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1691" spans="1:6" x14ac:dyDescent="0.25">
@@ -31477,16 +31513,16 @@
         <v>272</v>
       </c>
       <c r="B1691">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C1691">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1691">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1691">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1692" spans="1:6" x14ac:dyDescent="0.25">
@@ -31494,19 +31530,16 @@
         <v>272</v>
       </c>
       <c r="B1692">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C1692">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1692">
         <v>0</v>
       </c>
       <c r="E1692">
-        <v>3</v>
-      </c>
-      <c r="F1692" t="s">
-        <v>263</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1693" spans="1:6" x14ac:dyDescent="0.25">
@@ -31514,10 +31547,10 @@
         <v>272</v>
       </c>
       <c r="B1693">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C1693">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1693">
         <v>1</v>
@@ -31526,7 +31559,7 @@
         <v>3</v>
       </c>
       <c r="F1693" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
     </row>
     <row r="1694" spans="1:6" x14ac:dyDescent="0.25">
@@ -31534,16 +31567,16 @@
         <v>272</v>
       </c>
       <c r="B1694">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C1694">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1694">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1694">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1695" spans="1:6" x14ac:dyDescent="0.25">
@@ -31551,19 +31584,16 @@
         <v>272</v>
       </c>
       <c r="B1695">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C1695">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1695">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1695">
-        <v>4</v>
-      </c>
-      <c r="F1695" t="s">
-        <v>266</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1696" spans="1:6" x14ac:dyDescent="0.25">
@@ -31571,19 +31601,19 @@
         <v>272</v>
       </c>
       <c r="B1696">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C1696">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1696">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1696">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F1696" t="s">
-        <v>27</v>
+        <v>202</v>
       </c>
     </row>
     <row r="1697" spans="1:6" x14ac:dyDescent="0.25">
@@ -31591,19 +31621,16 @@
         <v>272</v>
       </c>
       <c r="B1697">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C1697">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D1697">
         <v>0</v>
       </c>
       <c r="E1697">
-        <v>5</v>
-      </c>
-      <c r="F1697" t="s">
-        <v>196</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1698" spans="1:6" x14ac:dyDescent="0.25">
@@ -31611,19 +31638,19 @@
         <v>272</v>
       </c>
       <c r="B1698">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C1698">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1698">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1698">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F1698" t="s">
-        <v>8</v>
+        <v>270</v>
       </c>
     </row>
     <row r="1699" spans="1:6" x14ac:dyDescent="0.25">
@@ -31631,16 +31658,19 @@
         <v>272</v>
       </c>
       <c r="B1699">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C1699">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1699">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1699">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="F1699" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="1700" spans="1:6" x14ac:dyDescent="0.25">
@@ -31648,19 +31678,16 @@
         <v>272</v>
       </c>
       <c r="B1700">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C1700">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1700">
         <v>0</v>
       </c>
       <c r="E1700">
-        <v>5</v>
-      </c>
-      <c r="F1700" t="s">
-        <v>267</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1701" spans="1:6" x14ac:dyDescent="0.25">
@@ -31668,19 +31695,16 @@
         <v>272</v>
       </c>
       <c r="B1701">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C1701">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1701">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1701">
-        <v>0</v>
-      </c>
-      <c r="F1701" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1702" spans="1:6" x14ac:dyDescent="0.25">
@@ -31688,7 +31712,7 @@
         <v>272</v>
       </c>
       <c r="B1702">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C1702">
         <v>0</v>
@@ -31698,9 +31722,6 @@
       </c>
       <c r="E1702">
         <v>0</v>
-      </c>
-      <c r="F1702" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="1703" spans="1:6" x14ac:dyDescent="0.25">
@@ -31708,19 +31729,16 @@
         <v>272</v>
       </c>
       <c r="B1703">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C1703">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1703">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1703">
-        <v>0</v>
-      </c>
-      <c r="F1703" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1704" spans="1:6" x14ac:dyDescent="0.25">
@@ -31728,16 +31746,16 @@
         <v>272</v>
       </c>
       <c r="B1704">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C1704">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1704">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1704">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1705" spans="1:6" x14ac:dyDescent="0.25">
@@ -31745,19 +31763,16 @@
         <v>272</v>
       </c>
       <c r="B1705">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C1705">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1705">
         <v>0</v>
       </c>
       <c r="E1705">
-        <v>2</v>
-      </c>
-      <c r="F1705" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1706" spans="1:6" x14ac:dyDescent="0.25">
@@ -31765,16 +31780,16 @@
         <v>272</v>
       </c>
       <c r="B1706">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C1706">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1706">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1706">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1707" spans="1:6" x14ac:dyDescent="0.25">
@@ -31782,19 +31797,16 @@
         <v>272</v>
       </c>
       <c r="B1707">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C1707">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1707">
         <v>0</v>
       </c>
       <c r="E1707">
-        <v>3</v>
-      </c>
-      <c r="F1707" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1708" spans="1:6" x14ac:dyDescent="0.25">
@@ -31802,19 +31814,16 @@
         <v>272</v>
       </c>
       <c r="B1708">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C1708">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1708">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1708">
-        <v>0</v>
-      </c>
-      <c r="F1708" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1709" spans="1:6" x14ac:dyDescent="0.25">
@@ -31822,7 +31831,7 @@
         <v>272</v>
       </c>
       <c r="B1709">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C1709">
         <v>0</v>
@@ -31832,6 +31841,9 @@
       </c>
       <c r="E1709">
         <v>0</v>
+      </c>
+      <c r="F1709" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="1710" spans="1:6" x14ac:dyDescent="0.25">
@@ -31839,19 +31851,16 @@
         <v>272</v>
       </c>
       <c r="B1710">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C1710">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1710">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1710">
-        <v>2</v>
-      </c>
-      <c r="F1710" t="s">
-        <v>268</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1711" spans="1:6" x14ac:dyDescent="0.25">
@@ -31859,16 +31868,16 @@
         <v>272</v>
       </c>
       <c r="B1711">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C1711">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1711">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1711">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1712" spans="1:6" x14ac:dyDescent="0.25">
@@ -31876,19 +31885,16 @@
         <v>272</v>
       </c>
       <c r="B1712">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C1712">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1712">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1712">
-        <v>5</v>
-      </c>
-      <c r="F1712" t="s">
-        <v>268</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1713" spans="1:6" x14ac:dyDescent="0.25">
@@ -31896,16 +31902,16 @@
         <v>272</v>
       </c>
       <c r="B1713">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C1713">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1713">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1713">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1714" spans="1:6" x14ac:dyDescent="0.25">
@@ -31913,16 +31919,16 @@
         <v>272</v>
       </c>
       <c r="B1714">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C1714">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1714">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1714">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1715" spans="1:6" x14ac:dyDescent="0.25">
@@ -31930,16 +31936,16 @@
         <v>272</v>
       </c>
       <c r="B1715">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C1715">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1715">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1715">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1716" spans="1:6" x14ac:dyDescent="0.25">
@@ -31947,16 +31953,16 @@
         <v>272</v>
       </c>
       <c r="B1716">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C1716">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1716">
         <v>1</v>
       </c>
       <c r="E1716">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1717" spans="1:6" x14ac:dyDescent="0.25">
@@ -31964,16 +31970,19 @@
         <v>272</v>
       </c>
       <c r="B1717">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C1717">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D1717">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1717">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="F1717" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="1718" spans="1:6" x14ac:dyDescent="0.25">
@@ -31981,10 +31990,10 @@
         <v>272</v>
       </c>
       <c r="B1718">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C1718">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D1718">
         <v>1</v>
@@ -31998,16 +32007,19 @@
         <v>272</v>
       </c>
       <c r="B1719">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C1719">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D1719">
         <v>0</v>
       </c>
       <c r="E1719">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="F1719" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="1720" spans="1:6" x14ac:dyDescent="0.25">
@@ -32015,16 +32027,16 @@
         <v>272</v>
       </c>
       <c r="B1720">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C1720">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1720">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1720">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1721" spans="1:6" x14ac:dyDescent="0.25">
@@ -32032,16 +32044,19 @@
         <v>272</v>
       </c>
       <c r="B1721">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C1721">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1721">
         <v>0</v>
       </c>
       <c r="E1721">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="F1721" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="1722" spans="1:6" x14ac:dyDescent="0.25">
@@ -32049,16 +32064,19 @@
         <v>272</v>
       </c>
       <c r="B1722">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C1722">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1722">
         <v>0</v>
       </c>
       <c r="E1722">
         <v>5</v>
+      </c>
+      <c r="F1722" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="1723" spans="1:6" x14ac:dyDescent="0.25">
@@ -32066,7 +32084,7 @@
         <v>272</v>
       </c>
       <c r="B1723">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C1723">
         <v>0</v>
@@ -32076,9 +32094,6 @@
       </c>
       <c r="E1723">
         <v>0</v>
-      </c>
-      <c r="F1723" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="1724" spans="1:6" x14ac:dyDescent="0.25">
@@ -32086,19 +32101,19 @@
         <v>272</v>
       </c>
       <c r="B1724">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="C1724">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1724">
         <v>0</v>
       </c>
       <c r="E1724">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F1724" t="s">
-        <v>12</v>
+        <v>263</v>
       </c>
     </row>
     <row r="1725" spans="1:6" x14ac:dyDescent="0.25">
@@ -32106,16 +32121,19 @@
         <v>272</v>
       </c>
       <c r="B1725">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="C1725">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1725">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1725">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="F1725" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="1726" spans="1:6" x14ac:dyDescent="0.25">
@@ -32123,16 +32141,16 @@
         <v>272</v>
       </c>
       <c r="B1726">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C1726">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1726">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1726">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1727" spans="1:6" x14ac:dyDescent="0.25">
@@ -32140,19 +32158,19 @@
         <v>272</v>
       </c>
       <c r="B1727">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C1727">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1727">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1727">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F1727" t="s">
-        <v>42</v>
+        <v>266</v>
       </c>
     </row>
     <row r="1728" spans="1:6" x14ac:dyDescent="0.25">
@@ -32160,16 +32178,19 @@
         <v>272</v>
       </c>
       <c r="B1728">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="C1728">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1728">
         <v>0</v>
       </c>
       <c r="E1728">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="F1728" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="1729" spans="1:6" x14ac:dyDescent="0.25">
@@ -32177,16 +32198,19 @@
         <v>272</v>
       </c>
       <c r="B1729">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="C1729">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1729">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1729">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="F1729" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="1730" spans="1:6" x14ac:dyDescent="0.25">
@@ -32194,19 +32218,19 @@
         <v>272</v>
       </c>
       <c r="B1730">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C1730">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1730">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1730">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F1730" t="s">
-        <v>256</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1731" spans="1:6" x14ac:dyDescent="0.25">
@@ -32214,7 +32238,7 @@
         <v>272</v>
       </c>
       <c r="B1731">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="C1731">
         <v>0</v>
@@ -32231,16 +32255,19 @@
         <v>272</v>
       </c>
       <c r="B1732">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="C1732">
         <v>1</v>
       </c>
       <c r="D1732">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1732">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="F1732" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="1733" spans="1:6" x14ac:dyDescent="0.25">
@@ -32248,7 +32275,7 @@
         <v>272</v>
       </c>
       <c r="B1733">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C1733">
         <v>0</v>
@@ -32258,6 +32285,9 @@
       </c>
       <c r="E1733">
         <v>0</v>
+      </c>
+      <c r="F1733" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="1734" spans="1:6" x14ac:dyDescent="0.25">
@@ -32265,16 +32295,19 @@
         <v>272</v>
       </c>
       <c r="B1734">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="C1734">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1734">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1734">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="F1734" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="1735" spans="1:6" x14ac:dyDescent="0.25">
@@ -32282,7 +32315,7 @@
         <v>272</v>
       </c>
       <c r="B1735">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C1735">
         <v>0</v>
@@ -32292,6 +32325,9 @@
       </c>
       <c r="E1735">
         <v>0</v>
+      </c>
+      <c r="F1735" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="1736" spans="1:6" x14ac:dyDescent="0.25">
@@ -32299,16 +32335,16 @@
         <v>272</v>
       </c>
       <c r="B1736">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C1736">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1736">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1736">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1737" spans="1:6" x14ac:dyDescent="0.25">
@@ -32316,16 +32352,19 @@
         <v>272</v>
       </c>
       <c r="B1737">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C1737">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1737">
         <v>0</v>
       </c>
       <c r="E1737">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="F1737" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="1738" spans="1:6" x14ac:dyDescent="0.25">
@@ -32333,19 +32372,16 @@
         <v>272</v>
       </c>
       <c r="B1738">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C1738">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1738">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1738">
-        <v>4</v>
-      </c>
-      <c r="F1738" t="s">
-        <v>257</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1739" spans="1:6" x14ac:dyDescent="0.25">
@@ -32353,16 +32389,19 @@
         <v>272</v>
       </c>
       <c r="B1739">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C1739">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1739">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1739">
         <v>3</v>
+      </c>
+      <c r="F1739" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="1740" spans="1:6" x14ac:dyDescent="0.25">
@@ -32370,19 +32409,19 @@
         <v>272</v>
       </c>
       <c r="B1740">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C1740">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D1740">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1740">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F1740" t="s">
-        <v>258</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1741" spans="1:6" x14ac:dyDescent="0.25">
@@ -32390,7 +32429,7 @@
         <v>272</v>
       </c>
       <c r="B1741">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C1741">
         <v>0</v>
@@ -32407,7 +32446,7 @@
         <v>272</v>
       </c>
       <c r="B1742">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C1742">
         <v>1</v>
@@ -32417,6 +32456,9 @@
       </c>
       <c r="E1742">
         <v>2</v>
+      </c>
+      <c r="F1742" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="1743" spans="1:6" x14ac:dyDescent="0.25">
@@ -32424,16 +32466,16 @@
         <v>272</v>
       </c>
       <c r="B1743">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C1743">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1743">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1743">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1744" spans="1:6" x14ac:dyDescent="0.25">
@@ -32441,16 +32483,19 @@
         <v>272</v>
       </c>
       <c r="B1744">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C1744">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1744">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1744">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="F1744" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="1745" spans="1:6" x14ac:dyDescent="0.25">
@@ -32458,16 +32503,16 @@
         <v>272</v>
       </c>
       <c r="B1745">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C1745">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1745">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1745">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1746" spans="1:6" x14ac:dyDescent="0.25">
@@ -32475,19 +32520,16 @@
         <v>272</v>
       </c>
       <c r="B1746">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C1746">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1746">
         <v>1</v>
       </c>
       <c r="E1746">
         <v>1</v>
-      </c>
-      <c r="F1746" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="1747" spans="1:6" x14ac:dyDescent="0.25">
@@ -32495,7 +32537,7 @@
         <v>272</v>
       </c>
       <c r="B1747">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C1747">
         <v>0</v>
@@ -32512,7 +32554,7 @@
         <v>272</v>
       </c>
       <c r="B1748">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C1748">
         <v>1</v>
@@ -32522,9 +32564,6 @@
       </c>
       <c r="E1748">
         <v>2</v>
-      </c>
-      <c r="F1748" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="1749" spans="1:6" x14ac:dyDescent="0.25">
@@ -32532,19 +32571,16 @@
         <v>272</v>
       </c>
       <c r="B1749">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C1749">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1749">
         <v>0</v>
       </c>
       <c r="E1749">
-        <v>2</v>
-      </c>
-      <c r="F1749" t="s">
-        <v>261</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1750" spans="1:6" x14ac:dyDescent="0.25">
@@ -32552,19 +32588,16 @@
         <v>272</v>
       </c>
       <c r="B1750">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C1750">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D1750">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1750">
-        <v>5</v>
-      </c>
-      <c r="F1750" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1751" spans="1:6" x14ac:dyDescent="0.25">
@@ -32572,16 +32605,16 @@
         <v>272</v>
       </c>
       <c r="B1751">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C1751">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D1751">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1751">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1752" spans="1:6" x14ac:dyDescent="0.25">
@@ -32589,19 +32622,16 @@
         <v>272</v>
       </c>
       <c r="B1752">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C1752">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D1752">
         <v>1</v>
       </c>
       <c r="E1752">
-        <v>5</v>
-      </c>
-      <c r="F1752" t="s">
-        <v>259</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1753" spans="1:6" x14ac:dyDescent="0.25">
@@ -32609,7 +32639,7 @@
         <v>272</v>
       </c>
       <c r="B1753">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C1753">
         <v>0</v>
@@ -32626,19 +32656,16 @@
         <v>272</v>
       </c>
       <c r="B1754">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C1754">
         <v>1</v>
       </c>
       <c r="D1754">
-        <v>1</v>
-      </c>
-      <c r="E1754" s="2">
+        <v>0</v>
+      </c>
+      <c r="E1754">
         <v>5</v>
-      </c>
-      <c r="F1754" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="1755" spans="1:6" x14ac:dyDescent="0.25">
@@ -32646,16 +32673,19 @@
         <v>272</v>
       </c>
       <c r="B1755">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C1755">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1755">
-        <v>1</v>
-      </c>
-      <c r="E1755" s="2">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="E1755">
+        <v>0</v>
+      </c>
+      <c r="F1755" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="1756" spans="1:6" x14ac:dyDescent="0.25">
@@ -32663,16 +32693,19 @@
         <v>272</v>
       </c>
       <c r="B1756">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C1756">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D1756">
-        <v>1</v>
-      </c>
-      <c r="E1756" s="2">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="E1756">
+        <v>0</v>
+      </c>
+      <c r="F1756" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="1757" spans="1:6" x14ac:dyDescent="0.25">
@@ -32680,7 +32713,7 @@
         <v>272</v>
       </c>
       <c r="B1757">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C1757">
         <v>0</v>
@@ -32688,7 +32721,7 @@
       <c r="D1757">
         <v>0</v>
       </c>
-      <c r="E1757" s="2">
+      <c r="E1757">
         <v>0</v>
       </c>
     </row>
@@ -32697,7 +32730,7 @@
         <v>272</v>
       </c>
       <c r="B1758">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C1758">
         <v>1</v>
@@ -32705,7 +32738,7 @@
       <c r="D1758">
         <v>1</v>
       </c>
-      <c r="E1758" s="2">
+      <c r="E1758">
         <v>1</v>
       </c>
     </row>
@@ -32714,16 +32747,19 @@
         <v>272</v>
       </c>
       <c r="B1759">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C1759">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1759">
-        <v>0</v>
-      </c>
-      <c r="E1759" s="2">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E1759">
+        <v>1</v>
+      </c>
+      <c r="F1759" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="1760" spans="1:6" x14ac:dyDescent="0.25">
@@ -32731,15 +32767,586 @@
         <v>272</v>
       </c>
       <c r="B1760">
+        <v>54</v>
+      </c>
+      <c r="C1760">
+        <v>0</v>
+      </c>
+      <c r="D1760">
+        <v>0</v>
+      </c>
+      <c r="E1760">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1761" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1761" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1761">
+        <v>54</v>
+      </c>
+      <c r="C1761">
+        <v>1</v>
+      </c>
+      <c r="D1761">
+        <v>1</v>
+      </c>
+      <c r="E1761">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1762" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1762" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1762">
+        <v>54</v>
+      </c>
+      <c r="C1762">
+        <v>2</v>
+      </c>
+      <c r="D1762">
+        <v>1</v>
+      </c>
+      <c r="E1762">
+        <v>1</v>
+      </c>
+      <c r="F1762" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="1763" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1763" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1763">
+        <v>55</v>
+      </c>
+      <c r="C1763">
+        <v>0</v>
+      </c>
+      <c r="D1763">
+        <v>0</v>
+      </c>
+      <c r="E1763">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1764" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1764" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1764">
+        <v>55</v>
+      </c>
+      <c r="C1764">
+        <v>1</v>
+      </c>
+      <c r="D1764">
+        <v>1</v>
+      </c>
+      <c r="E1764">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1765" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1765" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1765">
+        <v>56</v>
+      </c>
+      <c r="C1765">
+        <v>0</v>
+      </c>
+      <c r="D1765">
+        <v>0</v>
+      </c>
+      <c r="E1765">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1766" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1766" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1766">
+        <v>56</v>
+      </c>
+      <c r="C1766">
+        <v>1</v>
+      </c>
+      <c r="D1766">
+        <v>1</v>
+      </c>
+      <c r="E1766">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1767" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1767" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1767">
+        <v>57</v>
+      </c>
+      <c r="C1767">
+        <v>0</v>
+      </c>
+      <c r="D1767">
+        <v>0</v>
+      </c>
+      <c r="E1767">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1768" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1768" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1768">
+        <v>57</v>
+      </c>
+      <c r="C1768">
+        <v>1</v>
+      </c>
+      <c r="D1768">
+        <v>1</v>
+      </c>
+      <c r="E1768">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1769" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1769" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1769">
+        <v>58</v>
+      </c>
+      <c r="C1769">
+        <v>0</v>
+      </c>
+      <c r="D1769">
+        <v>0</v>
+      </c>
+      <c r="E1769">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1770" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1770" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1770">
+        <v>58</v>
+      </c>
+      <c r="C1770">
+        <v>1</v>
+      </c>
+      <c r="D1770">
+        <v>1</v>
+      </c>
+      <c r="E1770">
+        <v>4</v>
+      </c>
+      <c r="F1770" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="1771" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1771" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1771">
+        <v>58</v>
+      </c>
+      <c r="C1771">
+        <v>2</v>
+      </c>
+      <c r="D1771">
+        <v>1</v>
+      </c>
+      <c r="E1771">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1772" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1772" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1772">
+        <v>58</v>
+      </c>
+      <c r="C1772">
+        <v>3</v>
+      </c>
+      <c r="D1772">
+        <v>1</v>
+      </c>
+      <c r="E1772">
+        <v>2</v>
+      </c>
+      <c r="F1772" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="1773" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1773" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1773">
+        <v>59</v>
+      </c>
+      <c r="C1773">
+        <v>0</v>
+      </c>
+      <c r="D1773">
+        <v>0</v>
+      </c>
+      <c r="E1773">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1774" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1774" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1774">
+        <v>59</v>
+      </c>
+      <c r="C1774">
+        <v>1</v>
+      </c>
+      <c r="D1774">
+        <v>1</v>
+      </c>
+      <c r="E1774">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1775" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1775" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1775">
+        <v>59</v>
+      </c>
+      <c r="C1775">
+        <v>2</v>
+      </c>
+      <c r="D1775">
+        <v>1</v>
+      </c>
+      <c r="E1775">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1776" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1776" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1776">
+        <v>60</v>
+      </c>
+      <c r="C1776">
+        <v>0</v>
+      </c>
+      <c r="D1776">
+        <v>0</v>
+      </c>
+      <c r="E1776">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1777" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1777" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1777">
+        <v>60</v>
+      </c>
+      <c r="C1777">
+        <v>1</v>
+      </c>
+      <c r="D1777">
+        <v>1</v>
+      </c>
+      <c r="E1777">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1778" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1778" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1778">
+        <v>60</v>
+      </c>
+      <c r="C1778">
+        <v>2</v>
+      </c>
+      <c r="D1778">
+        <v>1</v>
+      </c>
+      <c r="E1778">
+        <v>1</v>
+      </c>
+      <c r="F1778" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="1779" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1779" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1779">
+        <v>61</v>
+      </c>
+      <c r="C1779">
+        <v>0</v>
+      </c>
+      <c r="D1779">
+        <v>0</v>
+      </c>
+      <c r="E1779">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1780" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1780" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1780">
+        <v>61</v>
+      </c>
+      <c r="C1780">
+        <v>1</v>
+      </c>
+      <c r="D1780">
+        <v>1</v>
+      </c>
+      <c r="E1780">
+        <v>2</v>
+      </c>
+      <c r="F1780" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="1781" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1781" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1781">
+        <v>61</v>
+      </c>
+      <c r="C1781">
+        <v>2</v>
+      </c>
+      <c r="D1781">
+        <v>0</v>
+      </c>
+      <c r="E1781">
+        <v>2</v>
+      </c>
+      <c r="F1781" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="1782" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1782" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1782">
+        <v>61</v>
+      </c>
+      <c r="C1782">
+        <v>3</v>
+      </c>
+      <c r="D1782">
+        <v>0</v>
+      </c>
+      <c r="E1782">
+        <v>5</v>
+      </c>
+      <c r="F1782" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="1783" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1783" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1783">
+        <v>61</v>
+      </c>
+      <c r="C1783">
+        <v>4</v>
+      </c>
+      <c r="D1783">
+        <v>1</v>
+      </c>
+      <c r="E1783">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1784" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1784" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1784">
+        <v>61</v>
+      </c>
+      <c r="C1784">
+        <v>5</v>
+      </c>
+      <c r="D1784">
+        <v>1</v>
+      </c>
+      <c r="E1784">
+        <v>5</v>
+      </c>
+      <c r="F1784" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="1785" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1785" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1785">
+        <v>62</v>
+      </c>
+      <c r="C1785">
+        <v>0</v>
+      </c>
+      <c r="D1785">
+        <v>0</v>
+      </c>
+      <c r="E1785">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1786" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1786" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1786">
+        <v>62</v>
+      </c>
+      <c r="C1786">
+        <v>1</v>
+      </c>
+      <c r="D1786">
+        <v>1</v>
+      </c>
+      <c r="E1786" s="2">
+        <v>5</v>
+      </c>
+      <c r="F1786" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="1787" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1787" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1787">
+        <v>62</v>
+      </c>
+      <c r="C1787">
+        <v>2</v>
+      </c>
+      <c r="D1787">
+        <v>1</v>
+      </c>
+      <c r="E1787" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1788" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1788" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1788">
+        <v>62</v>
+      </c>
+      <c r="C1788">
+        <v>3</v>
+      </c>
+      <c r="D1788">
+        <v>1</v>
+      </c>
+      <c r="E1788" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1789" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1789" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1789">
+        <v>63</v>
+      </c>
+      <c r="C1789">
+        <v>0</v>
+      </c>
+      <c r="D1789">
+        <v>0</v>
+      </c>
+      <c r="E1789" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1790" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1790" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1790">
+        <v>63</v>
+      </c>
+      <c r="C1790">
+        <v>1</v>
+      </c>
+      <c r="D1790">
+        <v>1</v>
+      </c>
+      <c r="E1790" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1791" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1791" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1791">
         <v>64</v>
       </c>
-      <c r="C1760">
-        <v>1</v>
-      </c>
-      <c r="D1760">
-        <v>1</v>
-      </c>
-      <c r="E1760" s="2">
+      <c r="C1791">
+        <v>0</v>
+      </c>
+      <c r="D1791">
+        <v>0</v>
+      </c>
+      <c r="E1791" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1792" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1792" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1792">
+        <v>64</v>
+      </c>
+      <c r="C1792">
+        <v>1</v>
+      </c>
+      <c r="D1792">
+        <v>1</v>
+      </c>
+      <c r="E1792" s="2">
         <v>1</v>
       </c>
     </row>
@@ -32753,7 +33360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C959004D-4D9F-441D-939C-D0A39F61DFAD}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -33005,7 +33612,7 @@
         <v>3</v>
       </c>
       <c r="H9">
-        <f>D9+E9+F9</f>
+        <f t="shared" ref="H9:H14" si="1">D9+E9+F9</f>
         <v>15</v>
       </c>
     </row>
@@ -33034,7 +33641,7 @@
         <v>1</v>
       </c>
       <c r="H10">
-        <f>D10+E10+F10</f>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
     </row>
@@ -33063,7 +33670,7 @@
         <v>12</v>
       </c>
       <c r="H11">
-        <f>D11+E11+F11</f>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="J11" t="s">
@@ -33095,7 +33702,7 @@
         <v>5</v>
       </c>
       <c r="H12">
-        <f>D12+E12+F12</f>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="J12" t="s">
@@ -33127,7 +33734,7 @@
         <v>2</v>
       </c>
       <c r="H13">
-        <f>D13+E13+F13</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
     </row>
@@ -33141,23 +33748,23 @@
       </c>
       <c r="C14">
         <f>COUNTIFS('Unit Info'!$A:$A,Summary!$A14,'Unit Info'!$E:$E,Summary!C$2,'Unit Info'!$D:$D, 1)</f>
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D14">
         <f>COUNTIFS('Unit Info'!$A:$A,Summary!$A14,'Unit Info'!$E:$E,Summary!D$2,'Unit Info'!$D:$D, 1)</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E14">
         <f>COUNTIFS('Unit Info'!$A:$A,Summary!$A14,'Unit Info'!$E:$E,Summary!E$2,'Unit Info'!$D:$D, 1)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F14">
         <f>COUNTIFS('Unit Info'!$A:$A,Summary!$A14,'Unit Info'!$E:$E,Summary!F$2,'Unit Info'!$D:$D, 1)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H14">
-        <f>D14+E14+F14</f>
-        <v>26</v>
+        <f t="shared" si="1"/>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update rf mapping for new mccartney data
</commit_message>
<xml_diff>
--- a/spike sorting notes.xlsx
+++ b/spike sorting notes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\MATLAB\gratings-task-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5F6F5E-107C-4D7B-9B71-AACA86159A24}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25329BF-FE75-4E2E-B935-1451CC28A9F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{F5215BA6-879C-42E2-A238-7256D4555DD7}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3660" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3664" uniqueCount="375">
   <si>
     <t>Session</t>
   </si>
@@ -1522,8 +1522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{991F1F63-41CC-4425-B140-2A823B1406A8}">
   <dimension ref="A1:H2824"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2801" workbookViewId="0">
-      <selection activeCell="H2823" sqref="H2823"/>
+    <sheetView tabSelected="1" topLeftCell="A2788" workbookViewId="0">
+      <selection activeCell="H2766" sqref="H2766"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36263,6 +36263,9 @@
       <c r="E1925">
         <v>0</v>
       </c>
+      <c r="H1925" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="1926" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1926" t="s">
@@ -36352,7 +36355,7 @@
         <v>0</v>
       </c>
       <c r="H1930" t="s">
-        <v>284</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1931" spans="1:8" x14ac:dyDescent="0.25">
@@ -36371,6 +36374,9 @@
       <c r="E1931">
         <v>0</v>
       </c>
+      <c r="H1931" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="1932" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1932" t="s">
@@ -36388,6 +36394,9 @@
       <c r="E1932">
         <v>0</v>
       </c>
+      <c r="H1932" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="1933" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1933" t="s">
@@ -36405,6 +36414,9 @@
       <c r="E1933">
         <v>0</v>
       </c>
+      <c r="H1933" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="1934" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1934" t="s">
@@ -52234,6 +52246,9 @@
       <c r="E2763">
         <v>0</v>
       </c>
+      <c r="H2763" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2764" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2764" t="s">
@@ -52290,9 +52305,6 @@
       </c>
       <c r="E2766">
         <v>0</v>
-      </c>
-      <c r="H2766" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2767" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update spike sorting notes
</commit_message>
<xml_diff>
--- a/spike sorting notes.xlsx
+++ b/spike sorting notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\MATLAB\gratings-task-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25329BF-FE75-4E2E-B935-1451CC28A9F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C70D37-4B76-4224-97D2-A1A18BCAC8A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{F5215BA6-879C-42E2-A238-7256D4555DD7}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3664" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3781" uniqueCount="386">
   <si>
     <t>Session</t>
   </si>
@@ -1157,6 +1157,39 @@
   <si>
     <t>Same ISI distribution as 4a, triphasic</t>
   </si>
+  <si>
+    <t>F20171002</t>
+  </si>
+  <si>
+    <t>Triphasic, changes in amplitude throughout session</t>
+  </si>
+  <si>
+    <t>Triphasic, probably same as 20a</t>
+  </si>
+  <si>
+    <t>same as 31a but more mixed in with noise cluster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double trough - combined early and late </t>
+  </si>
+  <si>
+    <t>Lots of drift</t>
+  </si>
+  <si>
+    <t>No clear, stable unit at times of interest</t>
+  </si>
+  <si>
+    <t>F20171004</t>
+  </si>
+  <si>
+    <t>May be triphasic</t>
+  </si>
+  <si>
+    <t>Broad trough. May be same as a</t>
+  </si>
+  <si>
+    <t>Bursty</t>
+  </si>
 </sst>
 </file>
 
@@ -1520,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{991F1F63-41CC-4425-B140-2A823B1406A8}">
-  <dimension ref="A1:H2824"/>
+  <dimension ref="A1:H2954"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2788" workbookViewId="0">
-      <selection activeCell="H2766" sqref="H2766"/>
+    <sheetView tabSelected="1" topLeftCell="A2305" workbookViewId="0">
+      <selection activeCell="D2333" sqref="D2333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44023,13 +44056,16 @@
         <v>2</v>
       </c>
       <c r="D2332">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2332">
         <v>3</v>
       </c>
       <c r="F2332">
         <v>8100</v>
+      </c>
+      <c r="H2332" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="2333" spans="1:8" x14ac:dyDescent="0.25">
@@ -53405,6 +53441,2459 @@
       </c>
       <c r="H2824" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="2825" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2825" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2825">
+        <v>1</v>
+      </c>
+      <c r="C2825">
+        <v>0</v>
+      </c>
+      <c r="D2825">
+        <v>0</v>
+      </c>
+      <c r="E2825">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2826" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2826" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2826">
+        <v>1</v>
+      </c>
+      <c r="C2826">
+        <v>1</v>
+      </c>
+      <c r="D2826">
+        <v>1</v>
+      </c>
+      <c r="E2826">
+        <v>3</v>
+      </c>
+      <c r="F2826">
+        <v>5400</v>
+      </c>
+      <c r="G2826">
+        <v>10800</v>
+      </c>
+      <c r="H2826" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="2827" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2827" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2827">
+        <v>1</v>
+      </c>
+      <c r="C2827">
+        <v>2</v>
+      </c>
+      <c r="D2827">
+        <v>1</v>
+      </c>
+      <c r="E2827">
+        <v>2</v>
+      </c>
+      <c r="F2827">
+        <v>5400</v>
+      </c>
+      <c r="G2827">
+        <v>6300</v>
+      </c>
+    </row>
+    <row r="2828" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2828" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2828">
+        <v>1</v>
+      </c>
+      <c r="C2828">
+        <v>3</v>
+      </c>
+      <c r="D2828">
+        <v>1</v>
+      </c>
+      <c r="E2828">
+        <v>2</v>
+      </c>
+      <c r="F2828">
+        <v>6300</v>
+      </c>
+      <c r="G2828">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="2829" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2829" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2829">
+        <v>2</v>
+      </c>
+      <c r="C2829">
+        <v>0</v>
+      </c>
+      <c r="D2829">
+        <v>0</v>
+      </c>
+      <c r="E2829">
+        <v>0</v>
+      </c>
+      <c r="H2829" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2830" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2830" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2830">
+        <v>3</v>
+      </c>
+      <c r="C2830">
+        <v>0</v>
+      </c>
+      <c r="D2830">
+        <v>0</v>
+      </c>
+      <c r="E2830">
+        <v>0</v>
+      </c>
+      <c r="H2830" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2831" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2831" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2831">
+        <v>4</v>
+      </c>
+      <c r="C2831">
+        <v>0</v>
+      </c>
+      <c r="D2831">
+        <v>0</v>
+      </c>
+      <c r="E2831">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2832" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2832" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2832">
+        <v>4</v>
+      </c>
+      <c r="C2832">
+        <v>1</v>
+      </c>
+      <c r="D2832">
+        <v>0</v>
+      </c>
+      <c r="E2832">
+        <v>4</v>
+      </c>
+      <c r="F2832">
+        <v>3600</v>
+      </c>
+      <c r="G2832">
+        <v>7200</v>
+      </c>
+      <c r="H2832" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2833" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2833" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2833">
+        <v>5</v>
+      </c>
+      <c r="C2833">
+        <v>0</v>
+      </c>
+      <c r="D2833">
+        <v>0</v>
+      </c>
+      <c r="E2833">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2834" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2834" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2834">
+        <v>5</v>
+      </c>
+      <c r="C2834">
+        <v>1</v>
+      </c>
+      <c r="D2834">
+        <v>1</v>
+      </c>
+      <c r="E2834">
+        <v>1</v>
+      </c>
+      <c r="F2834">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="2835" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2835" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2835">
+        <v>6</v>
+      </c>
+      <c r="C2835">
+        <v>0</v>
+      </c>
+      <c r="D2835">
+        <v>0</v>
+      </c>
+      <c r="E2835">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2836" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2836" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2836">
+        <v>6</v>
+      </c>
+      <c r="C2836">
+        <v>1</v>
+      </c>
+      <c r="D2836">
+        <v>0</v>
+      </c>
+      <c r="E2836">
+        <v>4</v>
+      </c>
+      <c r="F2836">
+        <v>1800</v>
+      </c>
+      <c r="G2836">
+        <v>4500</v>
+      </c>
+      <c r="H2836" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2837" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2837" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2837">
+        <v>7</v>
+      </c>
+      <c r="C2837">
+        <v>0</v>
+      </c>
+      <c r="D2837">
+        <v>0</v>
+      </c>
+      <c r="E2837">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2838" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2838" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2838">
+        <v>7</v>
+      </c>
+      <c r="C2838">
+        <v>1</v>
+      </c>
+      <c r="D2838">
+        <v>1</v>
+      </c>
+      <c r="E2838">
+        <v>3</v>
+      </c>
+      <c r="F2838">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="2839" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2839" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2839">
+        <v>8</v>
+      </c>
+      <c r="C2839">
+        <v>0</v>
+      </c>
+      <c r="D2839">
+        <v>0</v>
+      </c>
+      <c r="E2839">
+        <v>0</v>
+      </c>
+      <c r="H2839" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2840" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2840" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2840">
+        <v>9</v>
+      </c>
+      <c r="C2840">
+        <v>0</v>
+      </c>
+      <c r="D2840">
+        <v>0</v>
+      </c>
+      <c r="E2840">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2841" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2841" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2841">
+        <v>9</v>
+      </c>
+      <c r="C2841">
+        <v>1</v>
+      </c>
+      <c r="D2841">
+        <v>1</v>
+      </c>
+      <c r="E2841">
+        <v>3</v>
+      </c>
+      <c r="F2841">
+        <v>7200</v>
+      </c>
+      <c r="G2841">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="2842" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2842" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2842">
+        <v>10</v>
+      </c>
+      <c r="C2842">
+        <v>0</v>
+      </c>
+      <c r="D2842">
+        <v>0</v>
+      </c>
+      <c r="E2842">
+        <v>0</v>
+      </c>
+      <c r="H2842" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2843" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2843" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2843">
+        <v>11</v>
+      </c>
+      <c r="C2843">
+        <v>0</v>
+      </c>
+      <c r="D2843">
+        <v>0</v>
+      </c>
+      <c r="E2843">
+        <v>0</v>
+      </c>
+      <c r="H2843" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2844" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2844" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2844">
+        <v>12</v>
+      </c>
+      <c r="C2844">
+        <v>0</v>
+      </c>
+      <c r="D2844">
+        <v>0</v>
+      </c>
+      <c r="E2844">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2845" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2845" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2845">
+        <v>12</v>
+      </c>
+      <c r="C2845">
+        <v>1</v>
+      </c>
+      <c r="D2845">
+        <v>0</v>
+      </c>
+      <c r="E2845">
+        <v>4</v>
+      </c>
+      <c r="F2845">
+        <v>1800</v>
+      </c>
+      <c r="G2845">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="2846" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2846" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2846">
+        <v>12</v>
+      </c>
+      <c r="C2846">
+        <v>2</v>
+      </c>
+      <c r="D2846">
+        <v>0</v>
+      </c>
+      <c r="E2846">
+        <v>2</v>
+      </c>
+      <c r="F2846">
+        <v>3600</v>
+      </c>
+      <c r="H2846" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2847" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2847" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2847">
+        <v>13</v>
+      </c>
+      <c r="C2847">
+        <v>0</v>
+      </c>
+      <c r="D2847">
+        <v>0</v>
+      </c>
+      <c r="E2847">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2848" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2848" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2848">
+        <v>13</v>
+      </c>
+      <c r="C2848">
+        <v>1</v>
+      </c>
+      <c r="D2848">
+        <v>0</v>
+      </c>
+      <c r="E2848">
+        <v>2</v>
+      </c>
+      <c r="F2848">
+        <v>6300</v>
+      </c>
+      <c r="H2848" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2849" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2849" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2849">
+        <v>14</v>
+      </c>
+      <c r="C2849">
+        <v>0</v>
+      </c>
+      <c r="D2849">
+        <v>0</v>
+      </c>
+      <c r="E2849">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2850" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2850" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2850">
+        <v>14</v>
+      </c>
+      <c r="C2850">
+        <v>1</v>
+      </c>
+      <c r="D2850">
+        <v>0</v>
+      </c>
+      <c r="E2850">
+        <v>4</v>
+      </c>
+      <c r="F2850">
+        <v>6300</v>
+      </c>
+      <c r="H2850" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2851" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2851" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2851">
+        <v>15</v>
+      </c>
+      <c r="C2851">
+        <v>0</v>
+      </c>
+      <c r="D2851">
+        <v>0</v>
+      </c>
+      <c r="E2851">
+        <v>0</v>
+      </c>
+      <c r="H2851" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2852" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2852" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2852">
+        <v>16</v>
+      </c>
+      <c r="C2852">
+        <v>0</v>
+      </c>
+      <c r="D2852">
+        <v>0</v>
+      </c>
+      <c r="E2852">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2853" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2853" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2853">
+        <v>16</v>
+      </c>
+      <c r="C2853">
+        <v>1</v>
+      </c>
+      <c r="D2853">
+        <v>0</v>
+      </c>
+      <c r="E2853">
+        <v>5</v>
+      </c>
+      <c r="F2853">
+        <v>900</v>
+      </c>
+      <c r="G2853">
+        <v>1800</v>
+      </c>
+      <c r="H2853" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2854" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2854" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2854">
+        <v>17</v>
+      </c>
+      <c r="C2854">
+        <v>0</v>
+      </c>
+      <c r="D2854">
+        <v>0</v>
+      </c>
+      <c r="E2854">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2855" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2855" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2855">
+        <v>17</v>
+      </c>
+      <c r="C2855">
+        <v>1</v>
+      </c>
+      <c r="D2855">
+        <v>0</v>
+      </c>
+      <c r="E2855">
+        <v>2</v>
+      </c>
+      <c r="G2855">
+        <v>7200</v>
+      </c>
+      <c r="H2855" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2856" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2856" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2856">
+        <v>17</v>
+      </c>
+      <c r="C2856">
+        <v>2</v>
+      </c>
+      <c r="D2856">
+        <v>1</v>
+      </c>
+      <c r="E2856">
+        <v>3</v>
+      </c>
+      <c r="F2856">
+        <v>4500</v>
+      </c>
+      <c r="G2856">
+        <v>9900</v>
+      </c>
+    </row>
+    <row r="2857" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2857" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2857">
+        <v>17</v>
+      </c>
+      <c r="C2857">
+        <v>3</v>
+      </c>
+      <c r="D2857">
+        <v>0</v>
+      </c>
+      <c r="E2857">
+        <v>4</v>
+      </c>
+      <c r="F2857">
+        <v>9000</v>
+      </c>
+      <c r="H2857" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2858" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2858" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2858">
+        <v>18</v>
+      </c>
+      <c r="C2858">
+        <v>0</v>
+      </c>
+      <c r="D2858">
+        <v>0</v>
+      </c>
+      <c r="E2858">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2859" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2859" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2859">
+        <v>18</v>
+      </c>
+      <c r="C2859">
+        <v>1</v>
+      </c>
+      <c r="D2859">
+        <v>0</v>
+      </c>
+      <c r="E2859">
+        <v>4</v>
+      </c>
+      <c r="F2859">
+        <v>900</v>
+      </c>
+      <c r="G2859">
+        <v>2700</v>
+      </c>
+      <c r="H2859" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2860" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2860" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2860">
+        <v>18</v>
+      </c>
+      <c r="C2860">
+        <v>2</v>
+      </c>
+      <c r="D2860">
+        <v>0</v>
+      </c>
+      <c r="E2860">
+        <v>3</v>
+      </c>
+      <c r="F2860">
+        <v>2700</v>
+      </c>
+      <c r="G2860">
+        <v>6300</v>
+      </c>
+      <c r="H2860" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2861" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2861" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2861">
+        <v>19</v>
+      </c>
+      <c r="C2861">
+        <v>0</v>
+      </c>
+      <c r="D2861">
+        <v>0</v>
+      </c>
+      <c r="E2861">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2862" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2862" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2862">
+        <v>19</v>
+      </c>
+      <c r="C2862">
+        <v>1</v>
+      </c>
+      <c r="D2862">
+        <v>0</v>
+      </c>
+      <c r="E2862">
+        <v>4</v>
+      </c>
+      <c r="F2862">
+        <v>4500</v>
+      </c>
+      <c r="H2862" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2863" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2863" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2863">
+        <v>20</v>
+      </c>
+      <c r="C2863">
+        <v>0</v>
+      </c>
+      <c r="D2863">
+        <v>0</v>
+      </c>
+      <c r="E2863">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2864" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2864" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2864">
+        <v>20</v>
+      </c>
+      <c r="C2864">
+        <v>1</v>
+      </c>
+      <c r="D2864">
+        <v>0</v>
+      </c>
+      <c r="E2864">
+        <v>4</v>
+      </c>
+      <c r="G2864">
+        <v>7200</v>
+      </c>
+      <c r="H2864" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="2865" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2865" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2865">
+        <v>21</v>
+      </c>
+      <c r="C2865">
+        <v>0</v>
+      </c>
+      <c r="D2865">
+        <v>0</v>
+      </c>
+      <c r="E2865">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2866" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2866" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2866">
+        <v>21</v>
+      </c>
+      <c r="C2866">
+        <v>1</v>
+      </c>
+      <c r="D2866">
+        <v>0</v>
+      </c>
+      <c r="E2866">
+        <v>4</v>
+      </c>
+      <c r="G2866">
+        <v>900</v>
+      </c>
+      <c r="H2866" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="2867" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2867" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2867">
+        <v>22</v>
+      </c>
+      <c r="C2867">
+        <v>0</v>
+      </c>
+      <c r="D2867">
+        <v>0</v>
+      </c>
+      <c r="E2867">
+        <v>0</v>
+      </c>
+      <c r="H2867" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2868" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2868" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2868">
+        <v>23</v>
+      </c>
+      <c r="C2868">
+        <v>0</v>
+      </c>
+      <c r="D2868">
+        <v>0</v>
+      </c>
+      <c r="E2868">
+        <v>0</v>
+      </c>
+      <c r="H2868" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2869" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2869" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2869">
+        <v>24</v>
+      </c>
+      <c r="C2869">
+        <v>0</v>
+      </c>
+      <c r="D2869">
+        <v>0</v>
+      </c>
+      <c r="E2869">
+        <v>0</v>
+      </c>
+      <c r="H2869" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2870" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2870" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2870">
+        <v>25</v>
+      </c>
+      <c r="C2870">
+        <v>0</v>
+      </c>
+      <c r="D2870">
+        <v>0</v>
+      </c>
+      <c r="E2870">
+        <v>0</v>
+      </c>
+      <c r="H2870" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2871" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2871" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2871">
+        <v>26</v>
+      </c>
+      <c r="C2871">
+        <v>0</v>
+      </c>
+      <c r="D2871">
+        <v>0</v>
+      </c>
+      <c r="E2871">
+        <v>0</v>
+      </c>
+      <c r="H2871" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2872" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2872" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2872">
+        <v>27</v>
+      </c>
+      <c r="C2872">
+        <v>0</v>
+      </c>
+      <c r="D2872">
+        <v>0</v>
+      </c>
+      <c r="E2872">
+        <v>0</v>
+      </c>
+      <c r="H2872" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2873" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2873" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2873">
+        <v>28</v>
+      </c>
+      <c r="C2873">
+        <v>0</v>
+      </c>
+      <c r="D2873">
+        <v>0</v>
+      </c>
+      <c r="E2873">
+        <v>0</v>
+      </c>
+      <c r="H2873" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2874" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2874" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2874">
+        <v>29</v>
+      </c>
+      <c r="C2874">
+        <v>0</v>
+      </c>
+      <c r="D2874">
+        <v>0</v>
+      </c>
+      <c r="E2874">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2875" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2875" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2875">
+        <v>29</v>
+      </c>
+      <c r="C2875">
+        <v>1</v>
+      </c>
+      <c r="D2875">
+        <v>1</v>
+      </c>
+      <c r="E2875">
+        <v>2</v>
+      </c>
+      <c r="F2875">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="2876" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2876" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2876">
+        <v>30</v>
+      </c>
+      <c r="C2876">
+        <v>0</v>
+      </c>
+      <c r="D2876">
+        <v>0</v>
+      </c>
+      <c r="E2876">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2877" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2877" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2877">
+        <v>30</v>
+      </c>
+      <c r="C2877">
+        <v>1</v>
+      </c>
+      <c r="D2877">
+        <v>1</v>
+      </c>
+      <c r="E2877">
+        <v>2</v>
+      </c>
+      <c r="F2877">
+        <v>900</v>
+      </c>
+      <c r="G2877">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="2878" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2878" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2878">
+        <v>31</v>
+      </c>
+      <c r="C2878">
+        <v>0</v>
+      </c>
+      <c r="D2878">
+        <v>0</v>
+      </c>
+      <c r="E2878">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2879" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2879" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2879">
+        <v>31</v>
+      </c>
+      <c r="C2879">
+        <v>1</v>
+      </c>
+      <c r="D2879">
+        <v>1</v>
+      </c>
+      <c r="E2879">
+        <v>3</v>
+      </c>
+      <c r="F2879">
+        <v>7200</v>
+      </c>
+      <c r="G2879">
+        <v>9900</v>
+      </c>
+    </row>
+    <row r="2880" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2880" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2880">
+        <v>31</v>
+      </c>
+      <c r="C2880">
+        <v>2</v>
+      </c>
+      <c r="D2880">
+        <v>1</v>
+      </c>
+      <c r="E2880">
+        <v>2</v>
+      </c>
+      <c r="F2880">
+        <v>9900</v>
+      </c>
+      <c r="H2880" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="2881" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2881" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2881">
+        <v>32</v>
+      </c>
+      <c r="C2881">
+        <v>0</v>
+      </c>
+      <c r="D2881">
+        <v>0</v>
+      </c>
+      <c r="E2881">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2882" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2882" t="s">
+        <v>375</v>
+      </c>
+      <c r="B2882">
+        <v>32</v>
+      </c>
+      <c r="C2882">
+        <v>1</v>
+      </c>
+      <c r="D2882">
+        <v>1</v>
+      </c>
+      <c r="E2882">
+        <v>3</v>
+      </c>
+      <c r="F2882">
+        <v>6300</v>
+      </c>
+      <c r="H2882" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="2883" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2883" t="s">
+        <v>382</v>
+      </c>
+      <c r="B2883">
+        <v>1</v>
+      </c>
+      <c r="C2883">
+        <v>0</v>
+      </c>
+      <c r="D2883">
+        <v>0</v>
+      </c>
+      <c r="E2883">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2884" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2884">
+        <v>1</v>
+      </c>
+      <c r="C2884">
+        <v>1</v>
+      </c>
+      <c r="D2884">
+        <v>1</v>
+      </c>
+      <c r="E2884">
+        <v>4</v>
+      </c>
+      <c r="F2884">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="2885" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2885">
+        <v>1</v>
+      </c>
+      <c r="C2885">
+        <v>2</v>
+      </c>
+      <c r="D2885">
+        <v>1</v>
+      </c>
+      <c r="E2885">
+        <v>5</v>
+      </c>
+      <c r="F2885">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="2886" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2886">
+        <v>1</v>
+      </c>
+      <c r="C2886">
+        <v>3</v>
+      </c>
+      <c r="D2886">
+        <v>1</v>
+      </c>
+      <c r="E2886">
+        <v>3</v>
+      </c>
+      <c r="F2886">
+        <v>1800</v>
+      </c>
+      <c r="G2886">
+        <v>12600</v>
+      </c>
+    </row>
+    <row r="2887" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2887">
+        <v>1</v>
+      </c>
+      <c r="C2887">
+        <v>4</v>
+      </c>
+      <c r="D2887">
+        <v>1</v>
+      </c>
+      <c r="E2887">
+        <v>3</v>
+      </c>
+      <c r="F2887">
+        <v>2700</v>
+      </c>
+      <c r="G2887">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="2888" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2888">
+        <v>2</v>
+      </c>
+      <c r="C2888">
+        <v>0</v>
+      </c>
+      <c r="D2888">
+        <v>0</v>
+      </c>
+      <c r="E2888">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2889" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2889">
+        <v>2</v>
+      </c>
+      <c r="C2889">
+        <v>1</v>
+      </c>
+      <c r="D2889">
+        <v>1</v>
+      </c>
+      <c r="E2889">
+        <v>4</v>
+      </c>
+      <c r="F2889">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="2890" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2890">
+        <v>2</v>
+      </c>
+      <c r="C2890">
+        <v>2</v>
+      </c>
+      <c r="D2890">
+        <v>1</v>
+      </c>
+      <c r="E2890">
+        <v>4</v>
+      </c>
+      <c r="F2890">
+        <v>4500</v>
+      </c>
+      <c r="G2890">
+        <v>11700</v>
+      </c>
+      <c r="H2890" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="2891" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2891">
+        <v>2</v>
+      </c>
+      <c r="C2891">
+        <v>3</v>
+      </c>
+      <c r="D2891">
+        <v>1</v>
+      </c>
+      <c r="E2891">
+        <v>3</v>
+      </c>
+      <c r="F2891">
+        <v>11700</v>
+      </c>
+    </row>
+    <row r="2892" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2892">
+        <v>2</v>
+      </c>
+      <c r="C2892">
+        <v>4</v>
+      </c>
+      <c r="D2892">
+        <v>1</v>
+      </c>
+      <c r="E2892">
+        <v>3</v>
+      </c>
+      <c r="F2892">
+        <v>11700</v>
+      </c>
+    </row>
+    <row r="2893" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2893">
+        <v>3</v>
+      </c>
+      <c r="C2893">
+        <v>0</v>
+      </c>
+      <c r="D2893">
+        <v>0</v>
+      </c>
+      <c r="E2893">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2894" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2894">
+        <v>3</v>
+      </c>
+      <c r="C2894">
+        <v>1</v>
+      </c>
+      <c r="D2894">
+        <v>1</v>
+      </c>
+      <c r="E2894">
+        <v>2</v>
+      </c>
+      <c r="F2894">
+        <v>9900</v>
+      </c>
+    </row>
+    <row r="2895" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2895">
+        <v>4</v>
+      </c>
+      <c r="C2895">
+        <v>0</v>
+      </c>
+      <c r="D2895">
+        <v>0</v>
+      </c>
+      <c r="E2895">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2896" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2896">
+        <v>4</v>
+      </c>
+      <c r="C2896">
+        <v>1</v>
+      </c>
+      <c r="D2896">
+        <v>1</v>
+      </c>
+      <c r="E2896">
+        <v>1</v>
+      </c>
+      <c r="F2896">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="2897" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2897">
+        <v>5</v>
+      </c>
+      <c r="C2897">
+        <v>0</v>
+      </c>
+      <c r="D2897">
+        <v>0</v>
+      </c>
+      <c r="E2897">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2898" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2898">
+        <v>5</v>
+      </c>
+      <c r="C2898">
+        <v>1</v>
+      </c>
+      <c r="D2898">
+        <v>1</v>
+      </c>
+      <c r="E2898">
+        <v>3</v>
+      </c>
+      <c r="F2898">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="2899" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2899">
+        <v>6</v>
+      </c>
+      <c r="C2899">
+        <v>0</v>
+      </c>
+      <c r="D2899">
+        <v>0</v>
+      </c>
+      <c r="E2899">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2900" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2900">
+        <v>6</v>
+      </c>
+      <c r="C2900">
+        <v>1</v>
+      </c>
+      <c r="D2900">
+        <v>1</v>
+      </c>
+      <c r="E2900">
+        <v>2</v>
+      </c>
+      <c r="F2900">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="2901" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2901">
+        <v>7</v>
+      </c>
+      <c r="C2901">
+        <v>0</v>
+      </c>
+      <c r="D2901">
+        <v>0</v>
+      </c>
+      <c r="E2901">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2902" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2902">
+        <v>7</v>
+      </c>
+      <c r="C2902">
+        <v>1</v>
+      </c>
+      <c r="D2902">
+        <v>1</v>
+      </c>
+      <c r="E2902">
+        <v>3</v>
+      </c>
+      <c r="F2902">
+        <v>1800</v>
+      </c>
+      <c r="G2902">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="2903" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2903">
+        <v>7</v>
+      </c>
+      <c r="C2903">
+        <v>2</v>
+      </c>
+      <c r="D2903">
+        <v>1</v>
+      </c>
+      <c r="E2903">
+        <v>3</v>
+      </c>
+      <c r="F2903">
+        <v>2700</v>
+      </c>
+      <c r="G2903">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="2904" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2904">
+        <v>8</v>
+      </c>
+      <c r="C2904">
+        <v>0</v>
+      </c>
+      <c r="D2904">
+        <v>0</v>
+      </c>
+      <c r="E2904">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2905" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2905">
+        <v>8</v>
+      </c>
+      <c r="C2905">
+        <v>1</v>
+      </c>
+      <c r="D2905">
+        <v>1</v>
+      </c>
+      <c r="E2905">
+        <v>4</v>
+      </c>
+      <c r="F2905">
+        <v>1800</v>
+      </c>
+      <c r="H2905" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2906" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2906">
+        <v>8</v>
+      </c>
+      <c r="C2906">
+        <v>2</v>
+      </c>
+      <c r="D2906">
+        <v>1</v>
+      </c>
+      <c r="E2906">
+        <v>3</v>
+      </c>
+      <c r="F2906">
+        <v>2700</v>
+      </c>
+      <c r="G2906">
+        <v>13500</v>
+      </c>
+      <c r="H2906" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="2907" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2907">
+        <v>8</v>
+      </c>
+      <c r="C2907">
+        <v>3</v>
+      </c>
+      <c r="D2907">
+        <v>1</v>
+      </c>
+      <c r="E2907">
+        <v>3</v>
+      </c>
+      <c r="F2907">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="2908" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2908">
+        <v>8</v>
+      </c>
+      <c r="C2908">
+        <v>4</v>
+      </c>
+      <c r="D2908">
+        <v>1</v>
+      </c>
+      <c r="E2908">
+        <v>3</v>
+      </c>
+      <c r="F2908">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="2909" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2909">
+        <v>9</v>
+      </c>
+      <c r="C2909">
+        <v>0</v>
+      </c>
+      <c r="D2909">
+        <v>0</v>
+      </c>
+      <c r="E2909">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2910" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2910">
+        <v>9</v>
+      </c>
+      <c r="C2910">
+        <v>1</v>
+      </c>
+      <c r="D2910">
+        <v>1</v>
+      </c>
+      <c r="E2910">
+        <v>3</v>
+      </c>
+      <c r="F2910">
+        <v>14400</v>
+      </c>
+      <c r="H2910" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="2911" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2911">
+        <v>9</v>
+      </c>
+      <c r="C2911">
+        <v>2</v>
+      </c>
+      <c r="D2911">
+        <v>0</v>
+      </c>
+      <c r="E2911">
+        <v>3</v>
+      </c>
+      <c r="F2911">
+        <v>6300</v>
+      </c>
+      <c r="G2911">
+        <v>9000</v>
+      </c>
+      <c r="H2911" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2912" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2912">
+        <v>9</v>
+      </c>
+      <c r="C2912">
+        <v>3</v>
+      </c>
+      <c r="D2912">
+        <v>1</v>
+      </c>
+      <c r="E2912">
+        <v>3</v>
+      </c>
+      <c r="F2912">
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="2913" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2913">
+        <v>10</v>
+      </c>
+      <c r="C2913">
+        <v>0</v>
+      </c>
+      <c r="D2913">
+        <v>0</v>
+      </c>
+      <c r="E2913">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2914" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2914">
+        <v>10</v>
+      </c>
+      <c r="C2914">
+        <v>1</v>
+      </c>
+      <c r="D2914">
+        <v>0</v>
+      </c>
+      <c r="E2914">
+        <v>5</v>
+      </c>
+      <c r="F2914">
+        <v>7200</v>
+      </c>
+      <c r="G2914">
+        <v>13500</v>
+      </c>
+      <c r="H2914" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2915" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2915">
+        <v>10</v>
+      </c>
+      <c r="C2915">
+        <v>2</v>
+      </c>
+      <c r="D2915">
+        <v>1</v>
+      </c>
+      <c r="E2915">
+        <v>3</v>
+      </c>
+      <c r="F2915">
+        <v>11700</v>
+      </c>
+      <c r="H2915" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2916" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2916">
+        <v>11</v>
+      </c>
+      <c r="C2916">
+        <v>0</v>
+      </c>
+      <c r="D2916">
+        <v>0</v>
+      </c>
+      <c r="E2916">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2917" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2917">
+        <v>11</v>
+      </c>
+      <c r="C2917">
+        <v>1</v>
+      </c>
+      <c r="D2917">
+        <v>1</v>
+      </c>
+      <c r="E2917">
+        <v>3</v>
+      </c>
+      <c r="F2917">
+        <v>9900</v>
+      </c>
+    </row>
+    <row r="2918" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2918">
+        <v>11</v>
+      </c>
+      <c r="C2918">
+        <v>2</v>
+      </c>
+      <c r="D2918">
+        <v>1</v>
+      </c>
+      <c r="E2918">
+        <v>3</v>
+      </c>
+      <c r="F2918">
+        <v>9900</v>
+      </c>
+      <c r="H2918" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="2919" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2919">
+        <v>12</v>
+      </c>
+      <c r="C2919">
+        <v>0</v>
+      </c>
+      <c r="D2919">
+        <v>0</v>
+      </c>
+      <c r="E2919">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2920" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2920">
+        <v>12</v>
+      </c>
+      <c r="C2920">
+        <v>1</v>
+      </c>
+      <c r="D2920">
+        <v>1</v>
+      </c>
+      <c r="E2920">
+        <v>3</v>
+      </c>
+      <c r="F2920">
+        <v>5400</v>
+      </c>
+      <c r="G2920">
+        <v>9900</v>
+      </c>
+      <c r="H2920" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2921" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2921">
+        <v>13</v>
+      </c>
+      <c r="C2921">
+        <v>0</v>
+      </c>
+      <c r="D2921">
+        <v>0</v>
+      </c>
+      <c r="E2921">
+        <v>0</v>
+      </c>
+      <c r="H2921" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2922" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2922">
+        <v>14</v>
+      </c>
+      <c r="C2922">
+        <v>0</v>
+      </c>
+      <c r="D2922">
+        <v>0</v>
+      </c>
+      <c r="E2922">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2923" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2923">
+        <v>14</v>
+      </c>
+      <c r="C2923">
+        <v>1</v>
+      </c>
+      <c r="D2923">
+        <v>1</v>
+      </c>
+      <c r="E2923">
+        <v>3</v>
+      </c>
+      <c r="F2923">
+        <v>1800</v>
+      </c>
+      <c r="G2923">
+        <v>15300</v>
+      </c>
+      <c r="H2923" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2924" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2924">
+        <v>15</v>
+      </c>
+      <c r="C2924">
+        <v>0</v>
+      </c>
+      <c r="D2924">
+        <v>0</v>
+      </c>
+      <c r="E2924">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2925" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2925">
+        <v>15</v>
+      </c>
+      <c r="C2925">
+        <v>1</v>
+      </c>
+      <c r="D2925">
+        <v>1</v>
+      </c>
+      <c r="E2925">
+        <v>3</v>
+      </c>
+      <c r="F2925">
+        <v>6300</v>
+      </c>
+      <c r="G2925">
+        <v>10800</v>
+      </c>
+      <c r="H2925" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="2926" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2926">
+        <v>15</v>
+      </c>
+      <c r="C2926">
+        <v>2</v>
+      </c>
+      <c r="D2926">
+        <v>1</v>
+      </c>
+      <c r="E2926">
+        <v>5</v>
+      </c>
+      <c r="F2926">
+        <v>12600</v>
+      </c>
+      <c r="H2926" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2927" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2927">
+        <v>15</v>
+      </c>
+      <c r="C2927">
+        <v>3</v>
+      </c>
+      <c r="D2927">
+        <v>1</v>
+      </c>
+      <c r="E2927">
+        <v>3</v>
+      </c>
+      <c r="F2927">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="2928" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2928">
+        <v>16</v>
+      </c>
+      <c r="C2928">
+        <v>0</v>
+      </c>
+      <c r="D2928">
+        <v>0</v>
+      </c>
+      <c r="E2928">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2929" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2929">
+        <v>16</v>
+      </c>
+      <c r="C2929">
+        <v>1</v>
+      </c>
+      <c r="D2929">
+        <v>1</v>
+      </c>
+      <c r="E2929">
+        <v>4</v>
+      </c>
+      <c r="F2929">
+        <v>900</v>
+      </c>
+      <c r="G2929">
+        <v>6300</v>
+      </c>
+    </row>
+    <row r="2930" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2930">
+        <v>17</v>
+      </c>
+      <c r="C2930">
+        <v>0</v>
+      </c>
+      <c r="D2930">
+        <v>0</v>
+      </c>
+      <c r="E2930">
+        <v>0</v>
+      </c>
+      <c r="H2930" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2931" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2931">
+        <v>18</v>
+      </c>
+      <c r="C2931">
+        <v>0</v>
+      </c>
+      <c r="D2931">
+        <v>0</v>
+      </c>
+      <c r="E2931">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2932" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2932">
+        <v>18</v>
+      </c>
+      <c r="C2932">
+        <v>1</v>
+      </c>
+      <c r="D2932">
+        <v>0</v>
+      </c>
+      <c r="E2932">
+        <v>5</v>
+      </c>
+      <c r="F2932">
+        <v>12600</v>
+      </c>
+      <c r="H2932" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2933" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2933">
+        <v>19</v>
+      </c>
+      <c r="C2933">
+        <v>0</v>
+      </c>
+      <c r="D2933">
+        <v>0</v>
+      </c>
+      <c r="E2933">
+        <v>0</v>
+      </c>
+      <c r="H2933" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2934" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2934">
+        <v>20</v>
+      </c>
+      <c r="C2934">
+        <v>0</v>
+      </c>
+      <c r="D2934">
+        <v>0</v>
+      </c>
+      <c r="E2934">
+        <v>0</v>
+      </c>
+      <c r="H2934" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2935" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2935">
+        <v>21</v>
+      </c>
+      <c r="C2935">
+        <v>0</v>
+      </c>
+      <c r="D2935">
+        <v>0</v>
+      </c>
+      <c r="E2935">
+        <v>0</v>
+      </c>
+      <c r="H2935" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2936" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2936">
+        <v>22</v>
+      </c>
+      <c r="C2936">
+        <v>0</v>
+      </c>
+      <c r="D2936">
+        <v>0</v>
+      </c>
+      <c r="E2936">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2937" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2937">
+        <v>22</v>
+      </c>
+      <c r="C2937">
+        <v>1</v>
+      </c>
+      <c r="D2937">
+        <v>0</v>
+      </c>
+      <c r="E2937">
+        <v>3</v>
+      </c>
+      <c r="F2937">
+        <v>3600</v>
+      </c>
+      <c r="G2937">
+        <v>7200</v>
+      </c>
+      <c r="H2937" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2938" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2938">
+        <v>23</v>
+      </c>
+      <c r="C2938">
+        <v>0</v>
+      </c>
+      <c r="D2938">
+        <v>0</v>
+      </c>
+      <c r="E2938">
+        <v>0</v>
+      </c>
+      <c r="H2938" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2939" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2939">
+        <v>24</v>
+      </c>
+      <c r="C2939">
+        <v>0</v>
+      </c>
+      <c r="D2939">
+        <v>0</v>
+      </c>
+      <c r="E2939">
+        <v>0</v>
+      </c>
+      <c r="H2939" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2940" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2940">
+        <v>25</v>
+      </c>
+      <c r="C2940">
+        <v>0</v>
+      </c>
+      <c r="D2940">
+        <v>0</v>
+      </c>
+      <c r="E2940">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2941" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2941">
+        <v>25</v>
+      </c>
+      <c r="C2941">
+        <v>1</v>
+      </c>
+      <c r="D2941">
+        <v>1</v>
+      </c>
+      <c r="E2941">
+        <v>3</v>
+      </c>
+      <c r="F2941">
+        <v>2700</v>
+      </c>
+      <c r="H2941" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2942" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2942">
+        <v>26</v>
+      </c>
+      <c r="C2942">
+        <v>0</v>
+      </c>
+      <c r="D2942">
+        <v>0</v>
+      </c>
+      <c r="E2942">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2943" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2943">
+        <v>26</v>
+      </c>
+      <c r="C2943">
+        <v>1</v>
+      </c>
+      <c r="D2943">
+        <v>1</v>
+      </c>
+      <c r="E2943">
+        <v>2</v>
+      </c>
+      <c r="F2943">
+        <v>1800</v>
+      </c>
+      <c r="G2943">
+        <v>14400</v>
+      </c>
+    </row>
+    <row r="2944" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2944">
+        <v>26</v>
+      </c>
+      <c r="C2944">
+        <v>2</v>
+      </c>
+      <c r="D2944">
+        <v>0</v>
+      </c>
+      <c r="E2944">
+        <v>2</v>
+      </c>
+      <c r="F2944">
+        <v>7200</v>
+      </c>
+      <c r="H2944" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2945" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2945">
+        <v>27</v>
+      </c>
+      <c r="C2945">
+        <v>0</v>
+      </c>
+      <c r="D2945">
+        <v>0</v>
+      </c>
+      <c r="E2945">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2946" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2946">
+        <v>27</v>
+      </c>
+      <c r="C2946">
+        <v>1</v>
+      </c>
+      <c r="D2946">
+        <v>1</v>
+      </c>
+      <c r="E2946">
+        <v>2</v>
+      </c>
+      <c r="F2946">
+        <v>4500</v>
+      </c>
+      <c r="G2946">
+        <v>11700</v>
+      </c>
+    </row>
+    <row r="2947" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2947">
+        <v>28</v>
+      </c>
+      <c r="C2947">
+        <v>0</v>
+      </c>
+      <c r="D2947">
+        <v>0</v>
+      </c>
+      <c r="E2947">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2948" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2948">
+        <v>28</v>
+      </c>
+      <c r="C2948">
+        <v>1</v>
+      </c>
+      <c r="D2948">
+        <v>1</v>
+      </c>
+      <c r="E2948">
+        <v>3</v>
+      </c>
+      <c r="F2948">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="2949" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2949">
+        <v>29</v>
+      </c>
+      <c r="C2949">
+        <v>0</v>
+      </c>
+      <c r="D2949">
+        <v>0</v>
+      </c>
+      <c r="E2949">
+        <v>0</v>
+      </c>
+      <c r="H2949" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2950" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2950">
+        <v>30</v>
+      </c>
+      <c r="C2950">
+        <v>0</v>
+      </c>
+      <c r="D2950">
+        <v>0</v>
+      </c>
+      <c r="E2950">
+        <v>0</v>
+      </c>
+      <c r="H2950" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2951" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2951">
+        <v>31</v>
+      </c>
+      <c r="C2951">
+        <v>0</v>
+      </c>
+      <c r="D2951">
+        <v>0</v>
+      </c>
+      <c r="E2951">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2952" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2952">
+        <v>31</v>
+      </c>
+      <c r="C2952">
+        <v>1</v>
+      </c>
+      <c r="D2952">
+        <v>0</v>
+      </c>
+      <c r="E2952">
+        <v>4</v>
+      </c>
+      <c r="F2952">
+        <v>13500</v>
+      </c>
+      <c r="H2952" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2953" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2953">
+        <v>31</v>
+      </c>
+      <c r="C2953">
+        <v>2</v>
+      </c>
+      <c r="D2953">
+        <v>0</v>
+      </c>
+      <c r="E2953">
+        <v>4</v>
+      </c>
+      <c r="F2953">
+        <v>7200</v>
+      </c>
+      <c r="G2953">
+        <v>12600</v>
+      </c>
+      <c r="H2953" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2954" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2954">
+        <v>32</v>
+      </c>
+      <c r="C2954">
+        <v>0</v>
+      </c>
+      <c r="D2954">
+        <v>0</v>
+      </c>
+      <c r="E2954">
+        <v>0</v>
+      </c>
+      <c r="H2954" t="s">
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -53902,7 +56391,7 @@
       </c>
       <c r="D17">
         <f>COUNTIFS('Unit Info'!$A:$A,Summary!$A17,'Unit Info'!$E:$E,Summary!D$2,'Unit Info'!$D:$D, 1)</f>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E17">
         <f>COUNTIFS('Unit Info'!$A:$A,Summary!$A17,'Unit Info'!$E:$E,Summary!E$2,'Unit Info'!$D:$D, 1)</f>
@@ -53914,7 +56403,7 @@
       </c>
       <c r="H17">
         <f t="shared" ref="H17:H20" si="4">D17+E17+F17</f>
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>